<commit_message>
almost finish the dungeon gismo
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Dungeon.xlsx
+++ b/ConfigData/Xlsx/Dungeon.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -32,10 +32,6 @@
     <t>Id</t>
   </si>
   <si>
-    <t>Ename</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>string</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -97,6 +93,13 @@
   <si>
     <t>BgImage</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>t5</t>
   </si>
 </sst>
 </file>
@@ -1095,10 +1098,10 @@
   <autoFilter ref="A3:F7" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Ename" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{73907E41-59C0-4401-B513-FD3E83081BEC}" name="Des" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{D42DAE81-2DB3-494C-ACD3-312F37FCABDF}" name="EntryScene" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{15F66D07-23DA-465C-BEEA-DE826642173A}" name="Level" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{73907E41-59C0-4401-B513-FD3E83081BEC}" name="Des" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{D42DAE81-2DB3-494C-ACD3-312F37FCABDF}" name="EntryScene" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{15F66D07-23DA-465C-BEEA-DE826642173A}" name="Level" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{AF02DA69-E68C-4384-8DA2-96A94D0C4E76}" name="BgImage" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1429,7 +1432,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="F5" sqref="F5:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1446,19 +1449,19 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
@@ -1466,39 +1469,39 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>3</v>
+      <c r="B3" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
@@ -1506,7 +1509,7 @@
         <v>18000001</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8">
@@ -1515,8 +1518,8 @@
       <c r="E4" s="10">
         <v>3</v>
       </c>
-      <c r="F4" s="10">
-        <v>3</v>
+      <c r="F4" s="10" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
@@ -1524,7 +1527,7 @@
         <v>18000101</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8">
@@ -1533,8 +1536,8 @@
       <c r="E5" s="8">
         <v>8</v>
       </c>
-      <c r="F5" s="8">
-        <v>8</v>
+      <c r="F5" s="10" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
@@ -1542,7 +1545,7 @@
         <v>18000201</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8">
@@ -1551,8 +1554,8 @@
       <c r="E6" s="8">
         <v>5</v>
       </c>
-      <c r="F6" s="8">
-        <v>5</v>
+      <c r="F6" s="10" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
@@ -1560,7 +1563,7 @@
         <v>18000301</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8">
@@ -1569,8 +1572,8 @@
       <c r="E7" s="10">
         <v>10</v>
       </c>
-      <c r="F7" s="10">
-        <v>10</v>
+      <c r="F7" s="10" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
make uibutton differ in dungeon and common scene
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Dungeon.xlsx
+++ b/ConfigData/Xlsx/Dungeon.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -107,13 +107,57 @@
   </si>
   <si>
     <t>迷失森林入口十分显眼，其中也充满了诱惑。但是，很少有人有胆量进入其中。而那些真正进入其中的人，也极少能够平安返回。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Str</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Agi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intl</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>属性力量</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>属性敏捷</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>属性智慧</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>属性感知</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>属性耐力</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Perc</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Endu</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -311,7 +355,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -505,8 +549,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor theme="4"/>
       </patternFill>
     </fill>
   </fills>
@@ -774,7 +836,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -808,8 +870,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -856,7 +933,102 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1090,6 +1262,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1102,15 +1342,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:F7" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
-  <autoFilter ref="A3:F7" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{73907E41-59C0-4401-B513-FD3E83081BEC}" name="Des" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{D42DAE81-2DB3-494C-ACD3-312F37FCABDF}" name="EntryScene" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{15F66D07-23DA-465C-BEEA-DE826642173A}" name="Level" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{AF02DA69-E68C-4384-8DA2-96A94D0C4E76}" name="BgImage" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:K7" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+  <autoFilter ref="A3:K7"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="Id" dataDxfId="10"/>
+    <tableColumn id="2" name="Name" dataDxfId="9"/>
+    <tableColumn id="3" name="Des" dataDxfId="8"/>
+    <tableColumn id="9" name="EntryScene" dataDxfId="7"/>
+    <tableColumn id="10" name="Level" dataDxfId="6"/>
+    <tableColumn id="5" name="Str" dataDxfId="4"/>
+    <tableColumn id="7" name="Agi" dataDxfId="2"/>
+    <tableColumn id="6" name="Intl" dataDxfId="3"/>
+    <tableColumn id="8" name="Perc" dataDxfId="1"/>
+    <tableColumn id="11" name="Endu" dataDxfId="0"/>
+    <tableColumn id="4" name="BgImage" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1124,7 +1369,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1436,11 +1681,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1450,11 +1695,12 @@
     <col min="3" max="3" width="26.125" style="3" customWidth="1"/>
     <col min="4" max="4" width="9.5" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="3"/>
-    <col min="6" max="6" width="10.125" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="3"/>
+    <col min="6" max="10" width="5.625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="10.125" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1471,10 +1717,25 @@
         <v>11</v>
       </c>
       <c r="F1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1490,11 +1751,26 @@
       <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1510,11 +1786,26 @@
       <c r="E3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" s="7">
         <v>18000001</v>
       </c>
@@ -1530,11 +1821,16 @@
       <c r="E4" s="10">
         <v>3</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="7">
         <v>18000101</v>
       </c>
@@ -1548,11 +1844,16 @@
       <c r="E5" s="8">
         <v>8</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="7">
         <v>18000201</v>
       </c>
@@ -1566,11 +1867,16 @@
       <c r="E6" s="8">
         <v>5</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="7">
         <v>18000301</v>
       </c>
@@ -1584,7 +1890,12 @@
       <c r="E7" s="10">
         <v>10</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix the dungeon tansform bug
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Dungeon.xlsx
+++ b/ConfigData/Xlsx/Dungeon.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -151,6 +151,18 @@
   </si>
   <si>
     <t>Endu</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>出口地图</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExitScene</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -952,6 +964,16 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1047,16 +1069,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1342,20 +1354,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:K7" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
-  <autoFilter ref="A3:K7"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:L7" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+  <autoFilter ref="A3:L7"/>
+  <tableColumns count="12">
     <tableColumn id="1" name="Id" dataDxfId="10"/>
     <tableColumn id="2" name="Name" dataDxfId="9"/>
     <tableColumn id="3" name="Des" dataDxfId="8"/>
     <tableColumn id="9" name="EntryScene" dataDxfId="7"/>
+    <tableColumn id="12" name="ExitScene"/>
     <tableColumn id="10" name="Level" dataDxfId="6"/>
-    <tableColumn id="5" name="Str" dataDxfId="4"/>
-    <tableColumn id="7" name="Agi" dataDxfId="2"/>
+    <tableColumn id="5" name="Str" dataDxfId="5"/>
+    <tableColumn id="7" name="Agi" dataDxfId="4"/>
     <tableColumn id="6" name="Intl" dataDxfId="3"/>
-    <tableColumn id="8" name="Perc" dataDxfId="1"/>
-    <tableColumn id="11" name="Endu" dataDxfId="0"/>
-    <tableColumn id="4" name="BgImage" dataDxfId="5"/>
+    <tableColumn id="8" name="Perc" dataDxfId="2"/>
+    <tableColumn id="11" name="Endu" dataDxfId="1"/>
+    <tableColumn id="4" name="BgImage" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1682,10 +1695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1694,13 +1707,14 @@
     <col min="2" max="2" width="9" style="3"/>
     <col min="3" max="3" width="26.125" style="3" customWidth="1"/>
     <col min="4" max="4" width="9.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" style="3"/>
-    <col min="6" max="10" width="5.625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="10.125" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="3"/>
+    <col min="5" max="5" width="9.5" style="3" customWidth="1"/>
+    <col min="6" max="6" width="5.125" style="3" customWidth="1"/>
+    <col min="7" max="11" width="5.625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="10.125" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1714,28 +1728,31 @@
         <v>6</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="L1" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1749,10 +1766,10 @@
         <v>7</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>29</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>29</v>
@@ -1766,11 +1783,14 @@
       <c r="J2" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1784,28 +1804,31 @@
         <v>8</v>
       </c>
       <c r="E3" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="G3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="H3" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="I3" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="K3" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="L3" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" s="7">
         <v>18000001</v>
       </c>
@@ -1819,18 +1842,21 @@
         <v>13020001</v>
       </c>
       <c r="E4" s="10">
+        <v>13010002</v>
+      </c>
+      <c r="F4" s="10">
         <v>3</v>
       </c>
-      <c r="F4" s="10"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="10"/>
+      <c r="L4" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5" s="7">
         <v>18000101</v>
       </c>
@@ -1841,19 +1867,20 @@
       <c r="D5" s="8">
         <v>13020011</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="8"/>
+      <c r="F5" s="8">
         <v>8</v>
       </c>
-      <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="10"/>
+      <c r="L5" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6" s="7">
         <v>18000201</v>
       </c>
@@ -1864,19 +1891,20 @@
       <c r="D6" s="8">
         <v>13020021</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="8"/>
+      <c r="F6" s="8">
         <v>5</v>
       </c>
-      <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="10"/>
+      <c r="L6" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7" s="7">
         <v>18000301</v>
       </c>
@@ -1887,15 +1915,16 @@
       <c r="D7" s="8">
         <v>13020031</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="10"/>
+      <c r="F7" s="10">
         <v>10</v>
       </c>
-      <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="10" t="s">
+      <c r="K7" s="10"/>
+      <c r="L7" s="10" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add a attr test engine. fix a revive bug when in dungeon
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Dungeon.xlsx
+++ b/ConfigData/Xlsx/Dungeon.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1274,74 +1274,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1354,21 +1286,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:L7" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
-  <autoFilter ref="A3:L7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:L7" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+  <autoFilter ref="A3:L7" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Id" dataDxfId="10"/>
-    <tableColumn id="2" name="Name" dataDxfId="9"/>
-    <tableColumn id="3" name="Des" dataDxfId="8"/>
-    <tableColumn id="9" name="EntryScene" dataDxfId="7"/>
-    <tableColumn id="12" name="ExitScene"/>
-    <tableColumn id="10" name="Level" dataDxfId="6"/>
-    <tableColumn id="5" name="Str" dataDxfId="5"/>
-    <tableColumn id="7" name="Agi" dataDxfId="4"/>
-    <tableColumn id="6" name="Intl" dataDxfId="3"/>
-    <tableColumn id="8" name="Perc" dataDxfId="2"/>
-    <tableColumn id="11" name="Endu" dataDxfId="1"/>
-    <tableColumn id="4" name="BgImage" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Des" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="EntryScene" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="ExitScene"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Level" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Str" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Agi" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Intl" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Perc" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Endu" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="BgImage" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1382,7 +1314,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1694,11 +1626,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:K7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1877,7 +1809,9 @@
       <c r="D5" s="8">
         <v>13020011</v>
       </c>
-      <c r="E5" s="8"/>
+      <c r="E5" s="8">
+        <v>13010007</v>
+      </c>
       <c r="F5" s="8">
         <v>8</v>
       </c>
@@ -1911,7 +1845,9 @@
       <c r="D6" s="8">
         <v>13020021</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="8">
+        <v>13010004</v>
+      </c>
       <c r="F6" s="8">
         <v>5</v>
       </c>
@@ -1945,7 +1881,9 @@
       <c r="D7" s="8">
         <v>13020031</v>
       </c>
-      <c r="E7" s="10"/>
+      <c r="E7" s="10">
+        <v>13010005</v>
+      </c>
       <c r="F7" s="10">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
move the dungeon quest config to dungeon.xlsx
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Dungeon.xlsx
+++ b/ConfigData/Xlsx/Dungeon.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -164,6 +164,24 @@
   <si>
     <t>ExitScene</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>副本任务列表</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestDungeon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;4|manflower;2|sandland;2|cliff;2</t>
+  </si>
+  <si>
+    <t>trees;4|sandland;2|potteryroom;2|honeyhome;2|snare;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;4</t>
   </si>
 </sst>
 </file>
@@ -945,7 +963,26 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1286,21 +1323,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:L7" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
-  <autoFilter ref="A3:L7" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Des" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="EntryScene" dataDxfId="7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:M7" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="A3:M7" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Des" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="EntryScene" dataDxfId="8"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="ExitScene"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Level" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Str" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Agi" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Intl" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Perc" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Endu" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="BgImage" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Level" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Str" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Agi" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Intl" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Perc" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Endu" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{2CEA4510-7CD4-4840-B40D-96D33C618D34}" name="QuestDungeon" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="BgImage" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1627,10 +1665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1642,11 +1680,12 @@
     <col min="5" max="5" width="9.5" style="3" customWidth="1"/>
     <col min="6" max="6" width="5.125" style="3" customWidth="1"/>
     <col min="7" max="11" width="5.625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="10.125" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="3"/>
+    <col min="12" max="12" width="39.375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="10.125" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1680,11 +1719,14 @@
       <c r="K1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1718,11 +1760,14 @@
       <c r="K2" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="L2" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="M2" s="16" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1756,11 +1801,14 @@
       <c r="K3" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="L3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" s="7">
         <v>18000001</v>
       </c>
@@ -1795,10 +1843,13 @@
         <v>-1</v>
       </c>
       <c r="L4" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5" s="7">
         <v>18000101</v>
       </c>
@@ -1831,10 +1882,13 @@
         <v>-1</v>
       </c>
       <c r="L5" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A6" s="7">
         <v>18000201</v>
       </c>
@@ -1867,10 +1921,13 @@
         <v>-1</v>
       </c>
       <c r="L6" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7" s="7">
         <v>18000301</v>
       </c>
@@ -1903,6 +1960,9 @@
         <v>-1</v>
       </c>
       <c r="L7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="M7" s="10" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add a test scenequest. support mechanical move back
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Dungeon.xlsx
+++ b/ConfigData/Xlsx/Dungeon.xlsx
@@ -174,14 +174,15 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>trees;4|manflower;2|sandland;2|cliff;2</t>
-  </si>
-  <si>
     <t>trees;4|sandland;2|potteryroom;2|honeyhome;2|snare;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>trees;4</t>
+  </si>
+  <si>
+    <t>trees;4|manflower;2|sandland;2|cliff;2|losttree;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -982,6 +983,16 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1001,16 +1012,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1337,8 +1338,8 @@
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Intl" dataDxfId="4"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Perc" dataDxfId="3"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Endu" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{2CEA4510-7CD4-4840-B40D-96D33C618D34}" name="QuestDungeon" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="BgImage" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{2CEA4510-7CD4-4840-B40D-96D33C618D34}" name="QuestDungeon" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="BgImage" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1668,7 +1669,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1843,7 +1844,7 @@
         <v>-1</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="M4" s="10" t="s">
         <v>21</v>
@@ -1882,7 +1883,7 @@
         <v>-1</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M5" s="10" t="s">
         <v>20</v>
@@ -1921,7 +1922,7 @@
         <v>-1</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M6" s="10" t="s">
         <v>20</v>
@@ -1960,7 +1961,7 @@
         <v>-1</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M7" s="10" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
add some dungeon resource
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Dungeon.xlsx
+++ b/ConfigData/Xlsx/Dungeon.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -99,9 +99,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>t5</t>
-  </si>
-  <si>
     <t>losttrees</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -182,13 +179,35 @@
   </si>
   <si>
     <t>trees;4|manflower;2|river;2|cliff;2|losttree;2|oldtree;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>castle</t>
+  </si>
+  <si>
+    <t>viliage</t>
+  </si>
+  <si>
+    <t>tower</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>失落的古城，在城外就可以听到里面发出的各种奇怪的声音。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>这是一个废弃的村落，里面到底有什么样的东西呢。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>这是一个充满历史的高大建筑，里面蕴藏着许许多多不为人知的秘密</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1312,6 +1331,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1324,22 +1411,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:M7" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
-  <autoFilter ref="A3:M7" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:M7" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="A3:M7"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Des" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="EntryScene" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="ExitScene"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Level" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Str" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Agi" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Intl" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Perc" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Endu" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{2CEA4510-7CD4-4840-B40D-96D33C618D34}" name="QuestDungeon" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="BgImage" dataDxfId="0"/>
+    <tableColumn id="1" name="Id" dataDxfId="11"/>
+    <tableColumn id="2" name="Name" dataDxfId="10"/>
+    <tableColumn id="3" name="Des" dataDxfId="9"/>
+    <tableColumn id="9" name="EntryScene" dataDxfId="8"/>
+    <tableColumn id="12" name="ExitScene"/>
+    <tableColumn id="10" name="Level" dataDxfId="7"/>
+    <tableColumn id="5" name="Str" dataDxfId="6"/>
+    <tableColumn id="7" name="Agi" dataDxfId="5"/>
+    <tableColumn id="6" name="Intl" dataDxfId="4"/>
+    <tableColumn id="8" name="Perc" dataDxfId="3"/>
+    <tableColumn id="11" name="Endu" dataDxfId="2"/>
+    <tableColumn id="13" name="QuestDungeon" dataDxfId="1"/>
+    <tableColumn id="4" name="BgImage" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1353,7 +1440,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1665,11 +1752,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1700,28 +1787,28 @@
         <v>6</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="11" t="s">
-        <v>28</v>
-      </c>
       <c r="J1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="11" t="s">
-        <v>31</v>
-      </c>
       <c r="L1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M1" s="15" t="s">
         <v>17</v>
@@ -1741,25 +1828,25 @@
         <v>7</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>3</v>
@@ -1782,28 +1869,28 @@
         <v>8</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>12</v>
       </c>
       <c r="G3" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="I3" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="14" t="s">
-        <v>25</v>
-      </c>
       <c r="J3" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="14" t="s">
-        <v>33</v>
-      </c>
       <c r="L3" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M3" s="13" t="s">
         <v>18</v>
@@ -1817,7 +1904,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="8">
         <v>13020001</v>
@@ -1844,10 +1931,10 @@
         <v>-1</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.15">
@@ -1857,7 +1944,9 @@
       <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="8"/>
+      <c r="C5" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="D5" s="8">
         <v>13020011</v>
       </c>
@@ -1883,10 +1972,10 @@
         <v>-1</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.15">
@@ -1896,7 +1985,9 @@
       <c r="B6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="8" t="s">
+        <v>45</v>
+      </c>
       <c r="D6" s="8">
         <v>13020021</v>
       </c>
@@ -1922,10 +2013,10 @@
         <v>-1</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.15">
@@ -1935,7 +2026,9 @@
       <c r="B7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="D7" s="8">
         <v>13020031</v>
       </c>
@@ -1961,10 +2054,10 @@
         <v>-1</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add a new scenequest
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Dungeon.xlsx
+++ b/ConfigData/Xlsx/Dungeon.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -171,10 +171,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>trees;4|sandland;2|potteryroom;2|honeyhome;2|snare;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>trees;4</t>
   </si>
   <si>
@@ -201,13 +197,17 @@
   </si>
   <si>
     <t>这是一个充满历史的高大建筑，里面蕴藏着许许多多不为人知的秘密</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;2|sandland;2|potteryroom;2|honeyhome;2|snare;1|basement;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1331,74 +1331,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1411,22 +1343,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:M7" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
-  <autoFilter ref="A3:M7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:M7" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="A3:M7" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="Id" dataDxfId="11"/>
-    <tableColumn id="2" name="Name" dataDxfId="10"/>
-    <tableColumn id="3" name="Des" dataDxfId="9"/>
-    <tableColumn id="9" name="EntryScene" dataDxfId="8"/>
-    <tableColumn id="12" name="ExitScene"/>
-    <tableColumn id="10" name="Level" dataDxfId="7"/>
-    <tableColumn id="5" name="Str" dataDxfId="6"/>
-    <tableColumn id="7" name="Agi" dataDxfId="5"/>
-    <tableColumn id="6" name="Intl" dataDxfId="4"/>
-    <tableColumn id="8" name="Perc" dataDxfId="3"/>
-    <tableColumn id="11" name="Endu" dataDxfId="2"/>
-    <tableColumn id="13" name="QuestDungeon" dataDxfId="1"/>
-    <tableColumn id="4" name="BgImage" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Des" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="EntryScene" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="ExitScene"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Level" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Str" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Agi" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Intl" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Perc" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Endu" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="QuestDungeon" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="BgImage" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1440,7 +1372,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1752,11 +1684,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1931,7 +1863,7 @@
         <v>-1</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M4" s="10" t="s">
         <v>20</v>
@@ -1945,7 +1877,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" s="8">
         <v>13020011</v>
@@ -1972,10 +1904,10 @@
         <v>-1</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.15">
@@ -1986,7 +1918,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="8">
         <v>13020021</v>
@@ -1998,13 +1930,13 @@
         <v>5</v>
       </c>
       <c r="G6" s="10">
+        <v>2</v>
+      </c>
+      <c r="H6" s="10">
         <v>3</v>
       </c>
-      <c r="H6" s="10">
+      <c r="I6" s="10">
         <v>2</v>
-      </c>
-      <c r="I6" s="10">
-        <v>3</v>
       </c>
       <c r="J6" s="10">
         <v>-1</v>
@@ -2013,10 +1945,10 @@
         <v>-1</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.15">
@@ -2027,7 +1959,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="8">
         <v>13020031</v>
@@ -2054,10 +1986,10 @@
         <v>-1</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new scenequest func of item requirement
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Dungeon.xlsx
+++ b/ConfigData/Xlsx/Dungeon.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -200,14 +200,14 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>trees;2|sandland;2|potteryroom;2|honeyhome;2|snare;1|basement;1|woodhouse2;1|booty;1|trapspear;2|trapdrop;1</t>
+    <t>trees;2|sandland;2|potteryroom;2|honeyhome;2|snare;1|basement;1|woodhouse2;1|booty;1|trapspear;2|trapdrop;1|potteryman;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1343,22 +1343,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:M7" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
-  <autoFilter ref="A3:M7" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:M7" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="A3:M7"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Des" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="EntryScene" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="ExitScene"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Level" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Str" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Agi" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Intl" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Perc" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Endu" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="QuestDungeon" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="BgImage" dataDxfId="0"/>
+    <tableColumn id="1" name="Id" dataDxfId="11"/>
+    <tableColumn id="2" name="Name" dataDxfId="10"/>
+    <tableColumn id="3" name="Des" dataDxfId="9"/>
+    <tableColumn id="9" name="EntryScene" dataDxfId="8"/>
+    <tableColumn id="12" name="ExitScene"/>
+    <tableColumn id="10" name="Level" dataDxfId="7"/>
+    <tableColumn id="5" name="Str" dataDxfId="6"/>
+    <tableColumn id="7" name="Agi" dataDxfId="5"/>
+    <tableColumn id="6" name="Intl" dataDxfId="4"/>
+    <tableColumn id="8" name="Perc" dataDxfId="3"/>
+    <tableColumn id="11" name="Endu" dataDxfId="2"/>
+    <tableColumn id="13" name="QuestDungeon" dataDxfId="1"/>
+    <tableColumn id="4" name="BgImage" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1684,7 +1684,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>

<commit_message>
add some dungeon event
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Dungeon.xlsx
+++ b/ConfigData/Xlsx/Dungeon.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -200,14 +200,14 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>trees;2|sandland;2|potteryroom;2|honeyhome;2|snare;1|basement;1|woodhouse2;1|booty;1|trapspear;2|trapdrop;1|potteryman;1|stonedoor2;1</t>
+    <t>trees;2|sandland;2|potteryroom;2|honeyhome;2|snare;1|basement;1|woodhouse2;1|booty;1|trapspear;2|trapdrop;1|potteryman;1|stonedoor2;1|crystalball;2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1331,74 +1331,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1411,22 +1343,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:M7" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
-  <autoFilter ref="A3:M7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:M7" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="A3:M7" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="Id" dataDxfId="11"/>
-    <tableColumn id="2" name="Name" dataDxfId="10"/>
-    <tableColumn id="3" name="Des" dataDxfId="9"/>
-    <tableColumn id="9" name="EntryScene" dataDxfId="8"/>
-    <tableColumn id="12" name="ExitScene"/>
-    <tableColumn id="10" name="Level" dataDxfId="7"/>
-    <tableColumn id="5" name="Str" dataDxfId="6"/>
-    <tableColumn id="7" name="Agi" dataDxfId="5"/>
-    <tableColumn id="6" name="Intl" dataDxfId="4"/>
-    <tableColumn id="8" name="Perc" dataDxfId="3"/>
-    <tableColumn id="11" name="Endu" dataDxfId="2"/>
-    <tableColumn id="13" name="QuestDungeon" dataDxfId="1"/>
-    <tableColumn id="4" name="BgImage" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Des" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="EntryScene" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="ExitScene"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Level" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Str" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Agi" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Intl" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Perc" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Endu" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="QuestDungeon" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="BgImage" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1440,7 +1372,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1752,7 +1684,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>

<commit_message>
add some new quests
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Dungeon.xlsx
+++ b/ConfigData/Xlsx/Dungeon.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -174,10 +174,6 @@
     <t>trees;4</t>
   </si>
   <si>
-    <t>trees;4|manflower;2|river;2|cliff;2|losttree;2|oldtree;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>castle</t>
   </si>
   <si>
@@ -200,14 +196,18 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>trees;2|sandland;2|potteryroom;2|honeyhome;2|snare;1|basement;1|woodhouse2;1|booty;1|trapspear;2|trapdrop;1|potteryman;1|stonedoor2;1|crystalball;2</t>
+    <t>trees;4|manflower;2|river;2|cliff;2|losttree;2|oldtree;1|bookancient;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;2|sandland;2|potteryroom;2|honeyhome;2|snare;1|basement;1|woodhouse2;1|booty;1|trapspear;2|trapdrop;1|potteryman;1|stonedoor2;1|crystalball;2|bookancient;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1343,22 +1343,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:M7" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
-  <autoFilter ref="A3:M7" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:M7" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="A3:M7"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Des" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="EntryScene" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="ExitScene"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Level" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Str" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Agi" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Intl" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Perc" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Endu" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="QuestDungeon" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="BgImage" dataDxfId="0"/>
+    <tableColumn id="1" name="Id" dataDxfId="11"/>
+    <tableColumn id="2" name="Name" dataDxfId="10"/>
+    <tableColumn id="3" name="Des" dataDxfId="9"/>
+    <tableColumn id="9" name="EntryScene" dataDxfId="8"/>
+    <tableColumn id="12" name="ExitScene"/>
+    <tableColumn id="10" name="Level" dataDxfId="7"/>
+    <tableColumn id="5" name="Str" dataDxfId="6"/>
+    <tableColumn id="7" name="Agi" dataDxfId="5"/>
+    <tableColumn id="6" name="Intl" dataDxfId="4"/>
+    <tableColumn id="8" name="Perc" dataDxfId="3"/>
+    <tableColumn id="11" name="Endu" dataDxfId="2"/>
+    <tableColumn id="13" name="QuestDungeon" dataDxfId="1"/>
+    <tableColumn id="4" name="BgImage" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1684,11 +1684,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1863,7 +1863,7 @@
         <v>-1</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="M4" s="10" t="s">
         <v>20</v>
@@ -1877,7 +1877,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" s="8">
         <v>13020011</v>
@@ -1907,7 +1907,7 @@
         <v>38</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.15">
@@ -1918,7 +1918,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6" s="8">
         <v>13020021</v>
@@ -1948,7 +1948,7 @@
         <v>46</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.15">
@@ -1959,7 +1959,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="8">
         <v>13020031</v>
@@ -1989,7 +1989,7 @@
         <v>38</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new card event balance
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Dungeon.xlsx
+++ b/ConfigData/Xlsx/Dungeon.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -196,11 +196,26 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>trees;4|manflower;2|river;2|cliff;2|losttree;2|oldtree;1|bookancient;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trees;2|sandland;2|potteryroom;2|honeyhome;2|snare;1|basement;1|woodhouse2;1|booty;1|trapspear;2|trapdrop;1|potteryman;1|stonedoor2;1|crystalball;2|bookancient;1</t>
+    <t>bookancient;1</t>
+  </si>
+  <si>
+    <t>trees;2|sandland;2|potteryroom;2|honeyhome;2|snare;1|basement;1|woodhouse2;1|booty;1|trapspear;2|trapdrop;1|potteryman;1|stonedoor2;1|crystalball;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;4|manflower;2|river;2|cliff;2|losttree;2|oldtree;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestDungeonRate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bookdead;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bookancient;1|zookeeper;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -983,7 +998,26 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1343,22 +1377,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:M7" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
-  <autoFilter ref="A3:M7"/>
-  <tableColumns count="13">
-    <tableColumn id="1" name="Id" dataDxfId="11"/>
-    <tableColumn id="2" name="Name" dataDxfId="10"/>
-    <tableColumn id="3" name="Des" dataDxfId="9"/>
-    <tableColumn id="9" name="EntryScene" dataDxfId="8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:N7" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
+  <autoFilter ref="A3:N7"/>
+  <tableColumns count="14">
+    <tableColumn id="1" name="Id" dataDxfId="12"/>
+    <tableColumn id="2" name="Name" dataDxfId="11"/>
+    <tableColumn id="3" name="Des" dataDxfId="10"/>
+    <tableColumn id="9" name="EntryScene" dataDxfId="9"/>
     <tableColumn id="12" name="ExitScene"/>
-    <tableColumn id="10" name="Level" dataDxfId="7"/>
-    <tableColumn id="5" name="Str" dataDxfId="6"/>
-    <tableColumn id="7" name="Agi" dataDxfId="5"/>
-    <tableColumn id="6" name="Intl" dataDxfId="4"/>
-    <tableColumn id="8" name="Perc" dataDxfId="3"/>
-    <tableColumn id="11" name="Endu" dataDxfId="2"/>
-    <tableColumn id="13" name="QuestDungeon" dataDxfId="1"/>
-    <tableColumn id="4" name="BgImage" dataDxfId="0"/>
+    <tableColumn id="10" name="Level" dataDxfId="8"/>
+    <tableColumn id="5" name="Str" dataDxfId="7"/>
+    <tableColumn id="7" name="Agi" dataDxfId="6"/>
+    <tableColumn id="6" name="Intl" dataDxfId="5"/>
+    <tableColumn id="8" name="Perc" dataDxfId="4"/>
+    <tableColumn id="11" name="Endu" dataDxfId="3"/>
+    <tableColumn id="13" name="QuestDungeon" dataDxfId="2"/>
+    <tableColumn id="14" name="QuestDungeonRate" dataDxfId="0"/>
+    <tableColumn id="4" name="BgImage" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1685,10 +1720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1700,12 +1735,12 @@
     <col min="5" max="5" width="9.5" style="3" customWidth="1"/>
     <col min="6" max="6" width="5.125" style="3" customWidth="1"/>
     <col min="7" max="11" width="5.625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="39.375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="10.125" style="3" customWidth="1"/>
-    <col min="14" max="16384" width="9" style="3"/>
+    <col min="12" max="13" width="39.375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="10.125" style="3" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1742,11 +1777,14 @@
       <c r="L1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="M1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1783,11 +1821,14 @@
       <c r="L2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="M2" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="N2" s="16" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1824,11 +1865,14 @@
       <c r="L3" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="M3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="N3" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" s="7">
         <v>18000001</v>
       </c>
@@ -1863,13 +1907,16 @@
         <v>-1</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="M4" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="N4" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5" s="7">
         <v>18000101</v>
       </c>
@@ -1906,11 +1953,12 @@
       <c r="L5" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="M5" s="10"/>
+      <c r="N5" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6" s="7">
         <v>18000201</v>
       </c>
@@ -1948,10 +1996,13 @@
         <v>46</v>
       </c>
       <c r="M6" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="N6" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7" s="7">
         <v>18000301</v>
       </c>
@@ -1989,6 +2040,9 @@
         <v>38</v>
       </c>
       <c r="M7" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="N7" s="10" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
dungeon deck load from config
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Dungeon.xlsx
+++ b/ConfigData/Xlsx/Dungeon.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DBF21177-0899-42D1-BE7A-93B50C9CFF0D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -217,13 +218,28 @@
   </si>
   <si>
     <t>bookancient;1|safebox;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>默认卡组</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CardDeck</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dundefault</t>
+  </si>
+  <si>
+    <t>string</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -902,7 +918,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -953,6 +969,9 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -999,7 +1018,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="17">
     <dxf>
       <font>
         <b val="0"/>
@@ -1047,6 +1066,25 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1378,23 +1416,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:N7" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
-  <autoFilter ref="A3:N7"/>
-  <tableColumns count="14">
-    <tableColumn id="1" name="Id" dataDxfId="12"/>
-    <tableColumn id="2" name="Name" dataDxfId="11"/>
-    <tableColumn id="3" name="Des" dataDxfId="10"/>
-    <tableColumn id="9" name="EntryScene" dataDxfId="9"/>
-    <tableColumn id="12" name="ExitScene"/>
-    <tableColumn id="10" name="Level" dataDxfId="8"/>
-    <tableColumn id="5" name="Str" dataDxfId="7"/>
-    <tableColumn id="7" name="Agi" dataDxfId="6"/>
-    <tableColumn id="6" name="Intl" dataDxfId="5"/>
-    <tableColumn id="8" name="Perc" dataDxfId="4"/>
-    <tableColumn id="11" name="Endu" dataDxfId="3"/>
-    <tableColumn id="13" name="QuestDungeon" dataDxfId="2"/>
-    <tableColumn id="14" name="QuestDungeonRate" dataDxfId="0"/>
-    <tableColumn id="4" name="BgImage" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:O7" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" tableBorderDxfId="14">
+  <autoFilter ref="A3:O7" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Des" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="EntryScene" dataDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="ExitScene"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Level" dataDxfId="9"/>
+    <tableColumn id="15" xr3:uid="{6661BBD1-F9B6-46FD-93D8-A3785E2D75DD}" name="CardDeck" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Str" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Agi" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Intl" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Perc" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Endu" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="QuestDungeon" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="QuestDungeonRate" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="BgImage" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1720,11 +1759,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1735,13 +1774,14 @@
     <col min="4" max="4" width="9.5" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5" style="3" customWidth="1"/>
     <col min="6" max="6" width="5.125" style="3" customWidth="1"/>
-    <col min="7" max="11" width="5.625" style="3" customWidth="1"/>
-    <col min="12" max="13" width="39.375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="10.125" style="3" customWidth="1"/>
-    <col min="15" max="16384" width="9" style="3"/>
+    <col min="7" max="7" width="10.625" style="3" customWidth="1"/>
+    <col min="8" max="12" width="5.625" style="3" customWidth="1"/>
+    <col min="13" max="14" width="39.375" style="3" customWidth="1"/>
+    <col min="15" max="15" width="10.125" style="3" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1760,32 +1800,35 @@
       <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="N1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1804,8 +1847,8 @@
       <c r="F2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>28</v>
+      <c r="G2" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>28</v>
@@ -1819,17 +1862,20 @@
       <c r="K2" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="5" t="s">
-        <v>3</v>
+      <c r="L2" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="N2" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="O2" s="16" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1848,32 +1894,35 @@
       <c r="F3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="I3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="K3" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="L3" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="M3" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="N3" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="N3" s="13" t="s">
+      <c r="O3" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A4" s="7">
         <v>18000001</v>
       </c>
@@ -1892,32 +1941,35 @@
       <c r="F4" s="10">
         <v>3</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="10">
         <v>3</v>
       </c>
-      <c r="H4" s="10">
+      <c r="I4" s="10">
         <v>2</v>
       </c>
-      <c r="I4" s="10">
+      <c r="J4" s="10">
         <v>3</v>
-      </c>
-      <c r="J4" s="10">
-        <v>-1</v>
       </c>
       <c r="K4" s="10">
         <v>-1</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="10">
+        <v>-1</v>
+      </c>
+      <c r="M4" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="N4" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="O4" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A5" s="7">
         <v>18000101</v>
       </c>
@@ -1936,30 +1988,33 @@
       <c r="F5" s="8">
         <v>8</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="10">
         <v>3</v>
       </c>
-      <c r="H5" s="10">
+      <c r="I5" s="10">
         <v>2</v>
       </c>
-      <c r="I5" s="10">
+      <c r="J5" s="10">
         <v>3</v>
-      </c>
-      <c r="J5" s="10">
-        <v>-1</v>
       </c>
       <c r="K5" s="10">
         <v>-1</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="10">
+        <v>-1</v>
+      </c>
+      <c r="M5" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10" t="s">
+      <c r="N5" s="10"/>
+      <c r="O5" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6" s="7">
         <v>18000201</v>
       </c>
@@ -1978,32 +2033,35 @@
       <c r="F6" s="8">
         <v>5</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" s="10">
         <v>2</v>
       </c>
-      <c r="H6" s="10">
+      <c r="I6" s="10">
         <v>3</v>
       </c>
-      <c r="I6" s="10">
+      <c r="J6" s="10">
         <v>2</v>
-      </c>
-      <c r="J6" s="10">
-        <v>-1</v>
       </c>
       <c r="K6" s="10">
         <v>-1</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L6" s="10">
+        <v>-1</v>
+      </c>
+      <c r="M6" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="N6" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="O6" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A7" s="7">
         <v>18000301</v>
       </c>
@@ -2022,28 +2080,31 @@
       <c r="F7" s="10">
         <v>10</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" s="10">
         <v>3</v>
       </c>
-      <c r="H7" s="10">
+      <c r="I7" s="10">
         <v>2</v>
       </c>
-      <c r="I7" s="10">
+      <c r="J7" s="10">
         <v>3</v>
-      </c>
-      <c r="J7" s="10">
-        <v>-1</v>
       </c>
       <c r="K7" s="10">
         <v>-1</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="L7" s="10">
+        <v>-1</v>
+      </c>
+      <c r="M7" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="M7" s="10" t="s">
+      <c r="N7" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="N7" s="10" t="s">
+      <c r="O7" s="10" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add common fight event to dungeon
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Dungeon.xlsx
+++ b/ConfigData/Xlsx/Dungeon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DBF21177-0899-42D1-BE7A-93B50C9CFF0D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6214F650-2289-42CB-9987-D98E356486EC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -172,9 +172,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>trees;4</t>
-  </si>
-  <si>
     <t>castle</t>
   </si>
   <si>
@@ -197,14 +194,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>trees;2|sandland;2|potteryroom;2|honeyhome;2|snare;1|basement;1|woodhouse2;1|booty;1|trapspear;2|trapdrop;1|potteryman;1|stonedoor2;1|crystalball;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trees;4|manflower;2|river;2|cliff;2|losttree;2|oldtree;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>QuestDungeonRate</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -233,6 +222,18 @@
   </si>
   <si>
     <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fight;5|trees;4</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fight;7|trees;2|manflower;2|river;2|cliff;2|losttree;1|oldtree;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fight;10|sandland;2|potteryroom;2|honeyhome;2|snare;1|basement;1|woodhouse2;1|booty;1|trapspear;2|trapdrop;1|potteryman;1|stonedoor2;1|crystalball;2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1037,6 +1038,16 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1056,16 +1067,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1425,15 +1426,15 @@
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="EntryScene" dataDxfId="10"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="ExitScene"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Level" dataDxfId="9"/>
-    <tableColumn id="15" xr3:uid="{6661BBD1-F9B6-46FD-93D8-A3785E2D75DD}" name="CardDeck" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Str" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Agi" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Intl" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Perc" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Endu" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="QuestDungeon" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="QuestDungeonRate" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="BgImage" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{6661BBD1-F9B6-46FD-93D8-A3785E2D75DD}" name="CardDeck" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Str" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Agi" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Intl" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Perc" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Endu" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="QuestDungeon" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="QuestDungeonRate" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="BgImage" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1763,7 +1764,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1801,7 +1802,7 @@
         <v>11</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>25</v>
@@ -1848,7 +1849,7 @@
         <v>7</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>28</v>
@@ -1895,7 +1896,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H3" s="14" t="s">
         <v>22</v>
@@ -1916,7 +1917,7 @@
         <v>37</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="O3" s="13" t="s">
         <v>18</v>
@@ -1942,7 +1943,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H4" s="10">
         <v>3</v>
@@ -1960,10 +1961,10 @@
         <v>-1</v>
       </c>
       <c r="M4" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="N4" s="10" t="s">
         <v>46</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>49</v>
       </c>
       <c r="O4" s="10" t="s">
         <v>20</v>
@@ -1977,7 +1978,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="8">
         <v>13020011</v>
@@ -1989,7 +1990,7 @@
         <v>8</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H5" s="10">
         <v>3</v>
@@ -2007,11 +2008,11 @@
         <v>-1</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="N5" s="10"/>
       <c r="O5" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.15">
@@ -2022,7 +2023,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="8">
         <v>13020021</v>
@@ -2034,7 +2035,7 @@
         <v>5</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H6" s="10">
         <v>2</v>
@@ -2052,13 +2053,13 @@
         <v>-1</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="N6" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="O6" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.15">
@@ -2069,7 +2070,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" s="8">
         <v>13020031</v>
@@ -2081,7 +2082,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H7" s="10">
         <v>3</v>
@@ -2099,13 +2100,13 @@
         <v>-1</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove some cards events
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Dungeon.xlsx
+++ b/ConfigData/Xlsx/Dungeon.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6214F650-2289-42CB-9987-D98E356486EC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -202,10 +201,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>bookancient;1|zookeeper;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>bookancient;1|safebox;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -234,13 +229,17 @@
   </si>
   <si>
     <t>fight;10|sandland;2|potteryroom;2|honeyhome;2|snare;1|basement;1|woodhouse2;1|booty;1|trapspear;2|trapdrop;1|potteryman;1|stonedoor2;1|crystalball;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bookancient;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1405,6 +1404,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1417,24 +1484,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:O7" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" tableBorderDxfId="14">
-  <autoFilter ref="A3:O7" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:O7" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" tableBorderDxfId="14">
+  <autoFilter ref="A3:O7"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Des" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="EntryScene" dataDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="ExitScene"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Level" dataDxfId="9"/>
-    <tableColumn id="15" xr3:uid="{6661BBD1-F9B6-46FD-93D8-A3785E2D75DD}" name="CardDeck" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Str" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Agi" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Intl" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Perc" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Endu" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="QuestDungeon" dataDxfId="2"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="QuestDungeonRate" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="BgImage" dataDxfId="0"/>
+    <tableColumn id="1" name="Id" dataDxfId="13"/>
+    <tableColumn id="2" name="Name" dataDxfId="12"/>
+    <tableColumn id="3" name="Des" dataDxfId="11"/>
+    <tableColumn id="9" name="EntryScene" dataDxfId="10"/>
+    <tableColumn id="12" name="ExitScene"/>
+    <tableColumn id="10" name="Level" dataDxfId="9"/>
+    <tableColumn id="15" name="CardDeck" dataDxfId="8"/>
+    <tableColumn id="5" name="Str" dataDxfId="7"/>
+    <tableColumn id="7" name="Agi" dataDxfId="6"/>
+    <tableColumn id="6" name="Intl" dataDxfId="5"/>
+    <tableColumn id="8" name="Perc" dataDxfId="4"/>
+    <tableColumn id="11" name="Endu" dataDxfId="3"/>
+    <tableColumn id="13" name="QuestDungeon" dataDxfId="2"/>
+    <tableColumn id="14" name="QuestDungeonRate" dataDxfId="1"/>
+    <tableColumn id="4" name="BgImage" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1448,7 +1515,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1760,11 +1827,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1802,7 +1869,7 @@
         <v>11</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>25</v>
@@ -1849,7 +1916,7 @@
         <v>7</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>28</v>
@@ -1896,7 +1963,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H3" s="14" t="s">
         <v>22</v>
@@ -1943,7 +2010,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H4" s="10">
         <v>3</v>
@@ -1961,10 +2028,10 @@
         <v>-1</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N4" s="10" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="O4" s="10" t="s">
         <v>20</v>
@@ -1990,7 +2057,7 @@
         <v>8</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H5" s="10">
         <v>3</v>
@@ -2008,7 +2075,7 @@
         <v>-1</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N5" s="10"/>
       <c r="O5" s="10" t="s">
@@ -2035,7 +2102,7 @@
         <v>5</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H6" s="10">
         <v>2</v>
@@ -2053,10 +2120,10 @@
         <v>-1</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N6" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O6" s="10" t="s">
         <v>39</v>
@@ -2082,7 +2149,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H7" s="10">
         <v>3</v>
@@ -2100,7 +2167,7 @@
         <v>-1</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N7" s="10" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
add a dungeon card shop
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Dungeon.xlsx
+++ b/ConfigData/Xlsx/Dungeon.xlsx
@@ -228,11 +228,11 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>fight;10|sandland;2|potteryroom;2|honeyhome;2|snare;1|basement;1|woodhouse2;1|booty;1|trapspear;2|trapdrop;1|potteryman;1|stonedoor2;1|crystalball;2|cardbot;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>fight;7|trees;2|manflower;2|river;2|cliff;2|losttree;1|oldtree;1|cardbot;2</t>
+    <t>fight;7|trees;2|manflower;2|river;2|cliff;2|losttree;1|oldtree;1|cardbot;2|cardshop;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fight;10|sandland;2|potteryroom;2|honeyhome;2|snare;1|basement;1|woodhouse2;1|booty;1|trapspear;2|trapdrop;1|potteryman;1|stonedoor2;1|crystalball;2|cardbot;2|cardshop;2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2028,7 +2028,7 @@
         <v>-1</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N4" s="10" t="s">
         <v>52</v>
@@ -2120,7 +2120,7 @@
         <v>-1</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N6" s="10" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
can select job when enter dungeon
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Dungeon.xlsx
+++ b/ConfigData/Xlsx/Dungeon.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DB7428CC-5A3C-4787-BD74-DCB5FC1104D5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -233,13 +234,29 @@
   </si>
   <si>
     <t>fight;10|sandland;2|potteryroom;2|honeyhome;2|snare;1|basement;1|woodhouse2;1|booty;1|trapspear;2|trapdrop;1|potteryman;1|stonedoor2;1|crystalball;2|cardbot;2|cardshop;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>职业列表</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int[]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jobs</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>11000001;11000002;11000003</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1018,7 +1035,26 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1404,74 +1440,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1484,24 +1452,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:O7" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" tableBorderDxfId="14">
-  <autoFilter ref="A3:O7"/>
-  <tableColumns count="15">
-    <tableColumn id="1" name="Id" dataDxfId="13"/>
-    <tableColumn id="2" name="Name" dataDxfId="12"/>
-    <tableColumn id="3" name="Des" dataDxfId="11"/>
-    <tableColumn id="9" name="EntryScene" dataDxfId="10"/>
-    <tableColumn id="12" name="ExitScene"/>
-    <tableColumn id="10" name="Level" dataDxfId="9"/>
-    <tableColumn id="15" name="CardDeck" dataDxfId="8"/>
-    <tableColumn id="5" name="Str" dataDxfId="7"/>
-    <tableColumn id="7" name="Agi" dataDxfId="6"/>
-    <tableColumn id="6" name="Intl" dataDxfId="5"/>
-    <tableColumn id="8" name="Perc" dataDxfId="4"/>
-    <tableColumn id="11" name="Endu" dataDxfId="3"/>
-    <tableColumn id="13" name="QuestDungeon" dataDxfId="2"/>
-    <tableColumn id="14" name="QuestDungeonRate" dataDxfId="1"/>
-    <tableColumn id="4" name="BgImage" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:P7" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" tableBorderDxfId="15">
+  <autoFilter ref="A3:P7" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Des" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="EntryScene" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="ExitScene"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Level" dataDxfId="10"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="CardDeck" dataDxfId="9"/>
+    <tableColumn id="16" xr3:uid="{B81CDA0E-27DC-4980-96FC-17F047AF5C4F}" name="Jobs" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Str" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Agi" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Intl" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Perc" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Endu" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="QuestDungeon" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="QuestDungeonRate" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="BgImage" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1515,7 +1484,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1827,11 +1796,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="H4" sqref="H4:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1842,14 +1811,14 @@
     <col min="4" max="4" width="9.5" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5" style="3" customWidth="1"/>
     <col min="6" max="6" width="5.125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="10.625" style="3" customWidth="1"/>
-    <col min="8" max="12" width="5.625" style="3" customWidth="1"/>
-    <col min="13" max="14" width="39.375" style="3" customWidth="1"/>
-    <col min="15" max="15" width="10.125" style="3" customWidth="1"/>
-    <col min="16" max="16384" width="9" style="3"/>
+    <col min="7" max="8" width="10.625" style="3" customWidth="1"/>
+    <col min="9" max="13" width="5.625" style="3" customWidth="1"/>
+    <col min="14" max="15" width="39.375" style="3" customWidth="1"/>
+    <col min="16" max="16" width="10.125" style="3" customWidth="1"/>
+    <col min="17" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1871,32 +1840,35 @@
       <c r="G1" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="O1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1918,8 +1890,8 @@
       <c r="G2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>28</v>
+      <c r="H2" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>28</v>
@@ -1933,17 +1905,20 @@
       <c r="L2" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="5" t="s">
-        <v>3</v>
+      <c r="M2" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="16" t="s">
+      <c r="O2" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="P2" s="16" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1965,32 +1940,35 @@
       <c r="G3" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="K3" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="L3" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="M3" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="N3" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="O3" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="P3" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A4" s="7">
         <v>18000001</v>
       </c>
@@ -2012,32 +1990,35 @@
       <c r="G4" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" s="10">
         <v>3</v>
       </c>
-      <c r="I4" s="10">
+      <c r="J4" s="10">
         <v>2</v>
       </c>
-      <c r="J4" s="10">
+      <c r="K4" s="10">
         <v>3</v>
-      </c>
-      <c r="K4" s="10">
-        <v>-1</v>
       </c>
       <c r="L4" s="10">
         <v>-1</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="M4" s="10">
+        <v>-1</v>
+      </c>
+      <c r="N4" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="O4" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="O4" s="10" t="s">
+      <c r="P4" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A5" s="7">
         <v>18000101</v>
       </c>
@@ -2059,30 +2040,33 @@
       <c r="G5" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" s="10">
         <v>3</v>
       </c>
-      <c r="I5" s="10">
+      <c r="J5" s="10">
         <v>2</v>
       </c>
-      <c r="J5" s="10">
+      <c r="K5" s="10">
         <v>3</v>
-      </c>
-      <c r="K5" s="10">
-        <v>-1</v>
       </c>
       <c r="L5" s="10">
         <v>-1</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="M5" s="10">
+        <v>-1</v>
+      </c>
+      <c r="N5" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10" t="s">
+      <c r="O5" s="10"/>
+      <c r="P5" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A6" s="7">
         <v>18000201</v>
       </c>
@@ -2104,32 +2088,35 @@
       <c r="G6" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6" s="10">
         <v>2</v>
       </c>
-      <c r="I6" s="10">
+      <c r="J6" s="10">
         <v>3</v>
       </c>
-      <c r="J6" s="10">
+      <c r="K6" s="10">
         <v>2</v>
-      </c>
-      <c r="K6" s="10">
-        <v>-1</v>
       </c>
       <c r="L6" s="10">
         <v>-1</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="M6" s="10">
+        <v>-1</v>
+      </c>
+      <c r="N6" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="O6" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="O6" s="10" t="s">
+      <c r="P6" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A7" s="7">
         <v>18000301</v>
       </c>
@@ -2151,28 +2138,31 @@
       <c r="G7" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="10">
         <v>3</v>
       </c>
-      <c r="I7" s="10">
+      <c r="J7" s="10">
         <v>2</v>
       </c>
-      <c r="J7" s="10">
+      <c r="K7" s="10">
         <v>3</v>
-      </c>
-      <c r="K7" s="10">
-        <v>-1</v>
       </c>
       <c r="L7" s="10">
         <v>-1</v>
       </c>
-      <c r="M7" s="10" t="s">
+      <c r="M7" s="10">
+        <v>-1</v>
+      </c>
+      <c r="N7" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="N7" s="10" t="s">
+      <c r="O7" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="O7" s="10" t="s">
+      <c r="P7" s="10" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add the elite fight event
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Dungeon.xlsx
+++ b/ConfigData/Xlsx/Dungeon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DB7428CC-5A3C-4787-BD74-DCB5FC1104D5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F0FB15B1-362D-43BC-B9D0-BB11F3C2C0C2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -221,22 +221,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>fight;5|trees;4</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>bookancient;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>fight;7|trees;2|manflower;2|river;2|cliff;2|losttree;1|oldtree;1|cardbot;2|cardshop;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>fight;10|sandland;2|potteryroom;2|honeyhome;2|snare;1|basement;1|woodhouse2;1|booty;1|trapspear;2|trapdrop;1|potteryman;1|stonedoor2;1|crystalball;2|cardbot;2|cardshop;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>职业列表</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -250,6 +238,18 @@
   </si>
   <si>
     <t>11000001;11000002;11000003</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fight;7|fighte;2|trees;2|manflower;2|river;2|cliff;2|losttree;1|oldtree;1|cardbot;2|cardshop;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fight;5|fighte;2|trees;4</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fight;10|fighte;3|sandland;2|potteryroom;2|honeyhome;2|snare;1|basement;1|woodhouse2;1|booty;1|trapspear;2|trapdrop;1|potteryman;1|stonedoor2;1|crystalball;2|cardbot;2|cardshop;2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1054,6 +1054,16 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1073,16 +1083,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1462,15 +1462,15 @@
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="ExitScene"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Level" dataDxfId="10"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="CardDeck" dataDxfId="9"/>
-    <tableColumn id="16" xr3:uid="{B81CDA0E-27DC-4980-96FC-17F047AF5C4F}" name="Jobs" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Str" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Agi" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Intl" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Perc" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Endu" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="QuestDungeon" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="QuestDungeonRate" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="BgImage" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{B81CDA0E-27DC-4980-96FC-17F047AF5C4F}" name="Jobs" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Str" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Agi" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Intl" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Perc" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Endu" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="QuestDungeon" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="QuestDungeonRate" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="BgImage" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1800,7 +1800,7 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H7"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1841,7 +1841,7 @@
         <v>47</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>25</v>
@@ -1891,7 +1891,7 @@
         <v>50</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>28</v>
@@ -1941,7 +1941,7 @@
         <v>48</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I3" s="14" t="s">
         <v>22</v>
@@ -1991,7 +1991,7 @@
         <v>49</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I4" s="10">
         <v>3</v>
@@ -2009,10 +2009,10 @@
         <v>-1</v>
       </c>
       <c r="N4" s="10" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P4" s="10" t="s">
         <v>20</v>
@@ -2041,7 +2041,7 @@
         <v>49</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I5" s="10">
         <v>3</v>
@@ -2059,7 +2059,7 @@
         <v>-1</v>
       </c>
       <c r="N5" s="10" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="O5" s="10"/>
       <c r="P5" s="10" t="s">
@@ -2089,7 +2089,7 @@
         <v>49</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I6" s="10">
         <v>2</v>
@@ -2107,7 +2107,7 @@
         <v>-1</v>
       </c>
       <c r="N6" s="10" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="O6" s="10" t="s">
         <v>46</v>
@@ -2139,7 +2139,7 @@
         <v>49</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I7" s="10">
         <v>3</v>
@@ -2157,7 +2157,7 @@
         <v>-1</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="O7" s="10" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
optimise the count method of enemy and elite
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Dungeon.xlsx
+++ b/ConfigData/Xlsx/Dungeon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F0FB15B1-362D-43BC-B9D0-BB11F3C2C0C2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8B96E825-CD1E-48CD-BAB3-525E15490089}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,10 +100,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>losttrees</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>迷失森林入口十分显眼，其中也充满了诱惑。但是，很少有人有胆量进入其中。而那些真正进入其中的人，也极少能够平安返回。</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -241,16 +237,16 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>fight;7|fighte;2|trees;2|manflower;2|river;2|cliff;2|losttree;1|oldtree;1|cardbot;2|cardshop;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>fight;5|fighte;2|trees;4</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>fight;10|fighte;3|sandland;2|potteryroom;2|honeyhome;2|snare;1|basement;1|woodhouse2;1|booty;1|trapspear;2|trapdrop;1|potteryman;1|stonedoor2;1|crystalball;2|cardbot;2|cardshop;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
+    <t>lostftrees</t>
+  </si>
+  <si>
+    <t>fight;5|fighte;2|ftrees;4</t>
+  </si>
+  <si>
+    <t>fight;7|fighte;2|ftrees;2|emanflower;2|river;2|cliff;2|losttree;1|oldtree;1|cardbot;2|cardshop;2</t>
+  </si>
+  <si>
+    <t>fight;10|fighte;3|fsandland;2|potteryroom;2|fhoneyhome;2|esnare;1|basement;1|woodhouse2;1|ebooty;1|trapspear;2|trapdrop;1|potteryman;1|stonedoor2;1|crystalball;2|cardbot;2|cardshop;2</t>
   </si>
 </sst>
 </file>
@@ -1800,7 +1796,7 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1832,37 +1828,37 @@
         <v>6</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="11" t="s">
-        <v>27</v>
-      </c>
       <c r="L1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="11" t="s">
-        <v>30</v>
-      </c>
       <c r="N1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P1" s="15" t="s">
         <v>17</v>
@@ -1882,31 +1878,31 @@
         <v>7</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>3</v>
@@ -1932,37 +1928,37 @@
         <v>8</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>12</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I3" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="K3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="14" t="s">
-        <v>24</v>
-      </c>
       <c r="L3" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="14" t="s">
-        <v>32</v>
-      </c>
       <c r="N3" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P3" s="13" t="s">
         <v>18</v>
@@ -1976,7 +1972,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="8">
         <v>13020001</v>
@@ -1988,10 +1984,10 @@
         <v>3</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I4" s="10">
         <v>3</v>
@@ -2009,13 +2005,13 @@
         <v>-1</v>
       </c>
       <c r="N4" s="10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.15">
@@ -2026,7 +2022,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" s="8">
         <v>13020011</v>
@@ -2038,10 +2034,10 @@
         <v>8</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I5" s="10">
         <v>3</v>
@@ -2059,11 +2055,11 @@
         <v>-1</v>
       </c>
       <c r="N5" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O5" s="10"/>
       <c r="P5" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.15">
@@ -2074,7 +2070,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="8">
         <v>13020021</v>
@@ -2086,10 +2082,10 @@
         <v>5</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I6" s="10">
         <v>2</v>
@@ -2110,10 +2106,10 @@
         <v>58</v>
       </c>
       <c r="O6" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P6" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.15">
@@ -2124,7 +2120,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D7" s="8">
         <v>13020031</v>
@@ -2136,10 +2132,10 @@
         <v>10</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I7" s="10">
         <v>3</v>
@@ -2157,13 +2153,13 @@
         <v>-1</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P7" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
uniform the quest names
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Dungeon.xlsx
+++ b/ConfigData/Xlsx/Dungeon.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8B96E825-CD1E-48CD-BAB3-525E15490089}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -237,9 +236,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>lostftrees</t>
-  </si>
-  <si>
     <t>fight;5|fighte;2|ftrees;4</t>
   </si>
   <si>
@@ -247,12 +243,16 @@
   </si>
   <si>
     <t>fight;10|fighte;3|fsandland;2|potteryroom;2|fhoneyhome;2|esnare;1|basement;1|woodhouse2;1|ebooty;1|trapspear;2|trapdrop;1|potteryman;1|stonedoor2;1|crystalball;2|cardbot;2|cardshop;2</t>
+  </si>
+  <si>
+    <t>losttrees</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1436,6 +1436,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1448,25 +1516,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:P7" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" tableBorderDxfId="15">
-  <autoFilter ref="A3:P7" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:P7" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" tableBorderDxfId="15">
+  <autoFilter ref="A3:P7"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Des" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="EntryScene" dataDxfId="11"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="ExitScene"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Level" dataDxfId="10"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="CardDeck" dataDxfId="9"/>
-    <tableColumn id="16" xr3:uid="{B81CDA0E-27DC-4980-96FC-17F047AF5C4F}" name="Jobs" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Str" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Agi" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Intl" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Perc" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Endu" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="QuestDungeon" dataDxfId="2"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="QuestDungeonRate" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="BgImage" dataDxfId="0"/>
+    <tableColumn id="1" name="Id" dataDxfId="14"/>
+    <tableColumn id="2" name="Name" dataDxfId="13"/>
+    <tableColumn id="3" name="Des" dataDxfId="12"/>
+    <tableColumn id="9" name="EntryScene" dataDxfId="11"/>
+    <tableColumn id="12" name="ExitScene"/>
+    <tableColumn id="10" name="Level" dataDxfId="10"/>
+    <tableColumn id="15" name="CardDeck" dataDxfId="9"/>
+    <tableColumn id="16" name="Jobs" dataDxfId="8"/>
+    <tableColumn id="5" name="Str" dataDxfId="7"/>
+    <tableColumn id="7" name="Agi" dataDxfId="6"/>
+    <tableColumn id="6" name="Intl" dataDxfId="5"/>
+    <tableColumn id="8" name="Perc" dataDxfId="4"/>
+    <tableColumn id="11" name="Endu" dataDxfId="3"/>
+    <tableColumn id="13" name="QuestDungeon" dataDxfId="2"/>
+    <tableColumn id="14" name="QuestDungeonRate" dataDxfId="1"/>
+    <tableColumn id="4" name="BgImage" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1480,7 +1548,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1792,11 +1860,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2005,13 +2073,13 @@
         <v>-1</v>
       </c>
       <c r="N4" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O4" s="10" t="s">
         <v>50</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.15">
@@ -2055,7 +2123,7 @@
         <v>-1</v>
       </c>
       <c r="N5" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O5" s="10"/>
       <c r="P5" s="10" t="s">
@@ -2103,7 +2171,7 @@
         <v>-1</v>
       </c>
       <c r="N6" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O6" s="10" t="s">
         <v>45</v>
@@ -2153,7 +2221,7 @@
         <v>-1</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O7" s="10" t="s">
         <v>44</v>

</xml_diff>